<commit_message>
chore: JP tenth anni
</commit_message>
<xml_diff>
--- a/webcrawler/0_3_servents.xlsx
+++ b/webcrawler/0_3_servents.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2658,7 +2658,11 @@
           <t>Ｅ－フレアマリー</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Ｅ－火瑪麗</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr"/>
     </row>
     <row r="81">
@@ -2678,8 +2682,52 @@
           <t>Ｅ－アクアマリー</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Ｅ－水瑪麗</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>436</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Uolgamariegrandcollection</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Ｅ－グランマリー</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>443</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Uolgamariestellarcollection</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Ｅ－ステラマリー</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>